<commit_message>
added feature importance for all models
</commit_message>
<xml_diff>
--- a/Model_Results.xlsx
+++ b/Model_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nusu-my.sharepoint.com/personal/e0420265_u_nus_edu/Documents/School/BT4012/Project/Final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="478" documentId="8_{CEFDB902-4215-476E-846C-ABE7C069B124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74D09E25-67CF-434B-9A0A-4BA7B1DA7FA0}"/>
+  <xr:revisionPtr revIDLastSave="678" documentId="8_{CEFDB902-4215-476E-846C-ABE7C069B124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3BD7AF7-57EE-43C7-81AE-3CDC22685C84}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5666B08C-9E30-4A4A-A0C4-CA0B742E4B3B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5666B08C-9E30-4A4A-A0C4-CA0B742E4B3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Best" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="28">
   <si>
     <t>XGB</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>60% TRAINING DATA ON TEST DATA</t>
+  </si>
+  <si>
+    <t>40% TRAINING DATA ON TEST DATA</t>
+  </si>
+  <si>
+    <t>20% TRAINING DATA ON TEST DATA</t>
   </si>
 </sst>
 </file>
@@ -638,7 +644,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -808,6 +814,51 @@
     <xf numFmtId="10" fontId="2" fillId="6" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="7" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -820,15 +871,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -855,45 +897,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="7" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1210,10 +1213,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D7CCFF4-3E18-4F0A-B5C6-243756AF3955}">
-  <dimension ref="B1:Q34"/>
+  <dimension ref="B1:Q56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,27 +1231,27 @@
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" s="28"/>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="65" t="s">
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="65" t="s">
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="68"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="83"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="29" t="s">
@@ -1305,16 +1308,16 @@
         <v>0</v>
       </c>
       <c r="C4" s="18">
-        <v>0.19480519480519401</v>
+        <v>0.20091324200913199</v>
       </c>
       <c r="D4" s="26">
-        <v>0.25714285714285701</v>
+        <v>0.25492468134414797</v>
       </c>
       <c r="E4" s="19">
-        <v>0.27950310559006197</v>
+        <v>0.27329192546583803</v>
       </c>
       <c r="F4" s="45">
-        <v>0.50908902181158</v>
+        <v>0.50456708326768296</v>
       </c>
       <c r="G4" s="6">
         <v>9</v>
@@ -1335,19 +1338,19 @@
         <v>0.2</v>
       </c>
       <c r="M4" s="18">
-        <v>0.16501650165016499</v>
+        <v>0.18181818181818099</v>
       </c>
       <c r="N4" s="26">
-        <v>0.263991552270327</v>
+        <v>0.29411764705882298</v>
       </c>
       <c r="O4" s="19">
-        <v>0.31055900621117999</v>
+        <v>0.34782608695652101</v>
       </c>
       <c r="P4" s="45">
-        <v>0.52899057891551104</v>
+        <v>0.55995248500681205</v>
       </c>
       <c r="Q4" s="6">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
@@ -1435,16 +1438,16 @@
         <v>1</v>
       </c>
       <c r="M6" s="18">
-        <v>0.12698412698412601</v>
+        <v>0.126872246696035</v>
       </c>
       <c r="N6" s="26">
-        <v>0.40494938132733399</v>
+        <v>0.404721753794266</v>
       </c>
       <c r="O6" s="19">
         <v>0.894409937888198</v>
       </c>
       <c r="P6" s="45">
-        <v>0.74035061630875598</v>
+        <v>0.74011434675868004</v>
       </c>
       <c r="Q6" s="6">
         <v>0.7</v>
@@ -1455,49 +1458,49 @@
         <v>19</v>
       </c>
       <c r="C7" s="54">
-        <v>0.875</v>
+        <v>0.88888888888888795</v>
       </c>
       <c r="D7" s="55">
-        <v>5.3680981595091999E-2</v>
+        <v>6.1255742725880503E-2</v>
       </c>
       <c r="E7" s="56">
-        <v>4.3478260869565202E-2</v>
+        <v>4.9689440993788803E-2</v>
       </c>
       <c r="F7" s="59">
-        <v>0.20847363681720901</v>
+        <v>0.22286769232706799</v>
       </c>
       <c r="G7" s="57">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H7" s="54">
-        <v>0.46666666666666601</v>
+        <v>0.6</v>
       </c>
       <c r="I7" s="55">
-        <v>0.103857566765578</v>
+        <v>9.0361445783132502E-2</v>
       </c>
       <c r="J7" s="56">
-        <v>8.6956521739130405E-2</v>
+        <v>7.4534161490683204E-2</v>
       </c>
       <c r="K7" s="59">
-        <v>0.29395987114305999</v>
+        <v>0.27258204079420201</v>
       </c>
       <c r="L7" s="57">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="M7" s="54">
-        <v>0.14626865671641701</v>
+        <v>0.16927899686520301</v>
       </c>
       <c r="N7" s="55">
-        <v>0.25025536261491299</v>
+        <v>0.28037383177570002</v>
       </c>
       <c r="O7" s="56">
-        <v>0.30434782608695599</v>
+        <v>0.335403726708074</v>
       </c>
       <c r="P7" s="59">
-        <v>0.51991016079755403</v>
+        <v>0.54830964393270298</v>
       </c>
       <c r="Q7" s="57">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
@@ -1546,93 +1549,93 @@
       </c>
       <c r="C9" s="35">
         <f>AVERAGE(C4:C8)</f>
-        <v>0.33581608706153299</v>
+        <v>0.3408153210847395</v>
       </c>
       <c r="D9" s="36">
         <f>AVERAGE(D4:D8)</f>
-        <v>0.25897349945358478</v>
+        <v>0.26031264578660462</v>
       </c>
       <c r="E9" s="36">
         <f>AVERAGE(E4:E8)</f>
-        <v>0.39285714285714252</v>
+        <v>0.39285714285714246</v>
       </c>
       <c r="F9" s="60">
         <f>AVERAGE(F4:F8)</f>
-        <v>0.52051883358441697</v>
+        <v>0.52298686282590745</v>
       </c>
       <c r="G9" s="33"/>
       <c r="H9" s="35">
         <f>AVERAGE(H4:H8)</f>
-        <v>0.28255508571855659</v>
+        <v>0.30922175238522343</v>
       </c>
       <c r="I9" s="36">
         <f>AVERAGE(I4:I8)</f>
-        <v>0.2421443187257048</v>
+        <v>0.2394450945292157</v>
       </c>
       <c r="J9" s="36">
         <f>AVERAGE(J4:J8)</f>
-        <v>0.39751552795031031</v>
+        <v>0.39503105590062082</v>
       </c>
       <c r="K9" s="60">
         <f>AVERAGE(K4:K8)</f>
-        <v>0.50402876826207432</v>
+        <v>0.49975320219230285</v>
       </c>
       <c r="L9" s="33"/>
       <c r="M9" s="35">
         <f>AVERAGE(M4:M8)</f>
-        <v>0.14025448328289919</v>
+        <v>0.14819451128864142</v>
       </c>
       <c r="N9" s="36">
         <f>AVERAGE(N4:N8)</f>
-        <v>0.33566123547347082</v>
+        <v>0.34766462275671384</v>
       </c>
       <c r="O9" s="36">
         <f>AVERAGE(O4:O8)</f>
-        <v>0.60248447204968902</v>
+        <v>0.61614906832298089</v>
       </c>
       <c r="P9" s="60">
         <f>AVERAGE(P4:P8)</f>
-        <v>0.63971631571434562</v>
+        <v>0.65154133964962035</v>
       </c>
       <c r="Q9" s="33"/>
     </row>
     <row r="14" spans="2:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="87"/>
-      <c r="D14" s="87"/>
-      <c r="E14" s="87"/>
-      <c r="F14" s="87"/>
-      <c r="G14" s="87"/>
-      <c r="H14" s="87"/>
-      <c r="I14" s="87"/>
-      <c r="J14" s="87"/>
-      <c r="K14" s="87"/>
-      <c r="L14" s="87"/>
-      <c r="M14" s="87"/>
-      <c r="N14" s="87"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="76"/>
+      <c r="J14" s="76"/>
+      <c r="K14" s="76"/>
+      <c r="L14" s="76"/>
+      <c r="M14" s="76"/>
+      <c r="N14" s="76"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="28"/>
-      <c r="C15" s="69" t="s">
+      <c r="C15" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="69" t="s">
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="70"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="71"/>
-      <c r="K15" s="69" t="s">
+      <c r="H15" s="78"/>
+      <c r="I15" s="78"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="L15" s="70"/>
-      <c r="M15" s="70"/>
-      <c r="N15" s="71"/>
+      <c r="L15" s="78"/>
+      <c r="M15" s="78"/>
+      <c r="N15" s="79"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="29" t="s">
@@ -1680,16 +1683,16 @@
         <v>0</v>
       </c>
       <c r="C17" s="18">
-        <v>0.38461538461538403</v>
+        <v>0.22222222222222199</v>
       </c>
       <c r="D17" s="26">
-        <v>6.7750677506775006E-2</v>
+        <v>5.3475935828876997E-2</v>
       </c>
       <c r="E17" s="19">
-        <v>5.6179775280898799E-2</v>
+        <v>4.49438202247191E-2</v>
       </c>
       <c r="F17" s="62">
-        <v>0.236354590053175</v>
+        <v>0.21095265811633501</v>
       </c>
       <c r="G17" s="18">
         <v>0.17171717171717099</v>
@@ -1697,23 +1700,23 @@
       <c r="H17" s="26">
         <v>0.30685920577617298</v>
       </c>
-      <c r="I17" s="88">
+      <c r="I17" s="70">
         <v>0.38202247191011202</v>
       </c>
       <c r="J17" s="19">
         <v>0.58131971917178804</v>
       </c>
       <c r="K17" s="18">
-        <v>0.12555391432791699</v>
+        <v>0.122754491017964</v>
       </c>
       <c r="L17" s="26">
-        <v>0.41142303969022198</v>
-      </c>
-      <c r="M17" s="88">
-        <v>0.95505617977528001</v>
-      </c>
-      <c r="N17" s="90">
-        <v>0.74643962470129699</v>
+        <v>0.400390625</v>
+      </c>
+      <c r="M17" s="70">
+        <v>0.92134831460674105</v>
+      </c>
+      <c r="N17" s="72">
+        <v>0.73579718443313202</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
@@ -1738,7 +1741,7 @@
       <c r="H18" s="26">
         <v>0.40291262135922301</v>
       </c>
-      <c r="I18" s="88">
+      <c r="I18" s="70">
         <v>0.93258426966292096</v>
       </c>
       <c r="J18" s="19">
@@ -1750,10 +1753,10 @@
       <c r="L18" s="26">
         <v>0.412474849094567</v>
       </c>
-      <c r="M18" s="88">
+      <c r="M18" s="70">
         <v>0.92134831460674105</v>
       </c>
-      <c r="N18" s="90">
+      <c r="N18" s="72">
         <v>0.74889846019597694</v>
       </c>
     </row>
@@ -1774,16 +1777,16 @@
         <v>0</v>
       </c>
       <c r="G19" s="18">
-        <v>0.123493975903614</v>
+        <v>0.1236802413273</v>
       </c>
       <c r="H19" s="26">
-        <v>0.40196078431372501</v>
-      </c>
-      <c r="I19" s="88">
+        <v>0.40235525024533803</v>
+      </c>
+      <c r="I19" s="70">
         <v>0.92134831460674105</v>
       </c>
       <c r="J19" s="19">
-        <v>0.73755746729432203</v>
+        <v>0.73799688196975999</v>
       </c>
       <c r="K19" s="18">
         <v>0.125</v>
@@ -1791,10 +1794,10 @@
       <c r="L19" s="26">
         <v>0.40160642570281102</v>
       </c>
-      <c r="M19" s="88">
+      <c r="M19" s="70">
         <v>0.898876404494382</v>
       </c>
-      <c r="N19" s="90">
+      <c r="N19" s="72">
         <v>0.73799688196975999</v>
       </c>
     </row>
@@ -1811,32 +1814,32 @@
       <c r="E20" s="56">
         <v>2.2471910112359501E-2</v>
       </c>
-      <c r="F20" s="86">
+      <c r="F20" s="69">
         <v>0.14990633779917201</v>
       </c>
       <c r="G20" s="54">
-        <v>0.163265306122448</v>
+        <v>0.15075376884422101</v>
       </c>
       <c r="H20" s="55">
-        <v>0.28985507246376802</v>
-      </c>
-      <c r="I20" s="89">
-        <v>0.35955056179775202</v>
+        <v>0.27027027027027001</v>
+      </c>
+      <c r="I20" s="71">
+        <v>0.33707865168539303</v>
       </c>
       <c r="J20" s="56">
-        <v>0.56396296574110105</v>
+        <v>0.544967683583785</v>
       </c>
       <c r="K20" s="54">
-        <v>0.106353591160221</v>
+        <v>0.108381502890173</v>
       </c>
       <c r="L20" s="55">
-        <v>0.35648148148148101</v>
-      </c>
-      <c r="M20" s="89">
-        <v>0.86516853932584203</v>
-      </c>
-      <c r="N20" s="91">
-        <v>0.68647353770702102</v>
+        <v>0.35782442748091597</v>
+      </c>
+      <c r="M20" s="71">
+        <v>0.84269662921348298</v>
+      </c>
+      <c r="N20" s="73">
+        <v>0.69050465990731902</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
@@ -1852,7 +1855,7 @@
       <c r="E21" s="56">
         <v>4.49438202247191E-2</v>
       </c>
-      <c r="F21" s="86">
+      <c r="F21" s="69">
         <v>0.21140197206119801</v>
       </c>
       <c r="G21" s="54">
@@ -1861,7 +1864,7 @@
       <c r="H21" s="55">
         <v>0.360759493670886</v>
       </c>
-      <c r="I21" s="89">
+      <c r="I21" s="71">
         <v>0.64044943820224698</v>
       </c>
       <c r="J21" s="56">
@@ -1873,10 +1876,10 @@
       <c r="L21" s="55">
         <v>0.38877952755905498</v>
       </c>
-      <c r="M21" s="89">
+      <c r="M21" s="71">
         <v>0.88764044943820197</v>
       </c>
-      <c r="N21" s="91">
+      <c r="N21" s="73">
         <v>0.72437115222126602</v>
       </c>
     </row>
@@ -1897,28 +1900,28 @@
         <v>0</v>
       </c>
       <c r="G22" s="38">
-        <v>0.13763440860215001</v>
+        <v>0.137339055793991</v>
       </c>
       <c r="H22" s="39">
-        <v>0.38976857490864802</v>
+        <v>0.38929440389294401</v>
       </c>
       <c r="I22" s="39">
         <v>0.71910112359550504</v>
       </c>
       <c r="J22" s="40">
-        <v>0.71845245078893505</v>
+        <v>0.71810018185342095</v>
       </c>
       <c r="K22" s="38">
-        <v>0.123711340206185</v>
+        <v>0.121700879765395</v>
       </c>
       <c r="L22" s="39">
-        <v>0.405797101449275</v>
+        <v>0.399807321772639</v>
       </c>
       <c r="M22" s="39">
-        <v>0.94382022471910099</v>
-      </c>
-      <c r="N22" s="92">
-        <v>0.74069194954612005</v>
+        <v>0.93258426966292096</v>
+      </c>
+      <c r="N22" s="74">
+        <v>0.73448496925763596</v>
       </c>
     </row>
     <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1927,90 +1930,90 @@
       </c>
       <c r="C23" s="35">
         <f>AVERAGE(C17:C22)</f>
-        <v>0.45299145299145288</v>
+        <v>0.42592592592592582</v>
       </c>
       <c r="D23" s="36">
         <f t="shared" ref="D23:N23" si="0">AVERAGE(D17:D22)</f>
-        <v>2.7339511121413751E-2</v>
+        <v>2.4960387508430753E-2</v>
       </c>
       <c r="E23" s="36">
         <f t="shared" si="0"/>
-        <v>2.2471910112359519E-2</v>
+        <v>2.0599250936329565E-2</v>
       </c>
       <c r="F23" s="64">
         <f t="shared" si="0"/>
-        <v>0.1172771146523635</v>
+        <v>0.11304345932955684</v>
       </c>
       <c r="G23" s="35">
         <f>AVERAGE(G17:G22)</f>
-        <v>0.14176544474480116</v>
+        <v>0.13966200730101783</v>
       </c>
       <c r="H23" s="36">
         <f t="shared" si="0"/>
-        <v>0.35868595874873721</v>
+        <v>0.35540854086913898</v>
       </c>
       <c r="I23" s="36">
         <f t="shared" si="0"/>
-        <v>0.65917602996254632</v>
+        <v>0.6554307116104866</v>
       </c>
       <c r="J23" s="64">
         <f t="shared" si="0"/>
-        <v>0.6708830113580716</v>
+        <v>0.66773165528850609</v>
       </c>
       <c r="K23" s="35">
         <f>AVERAGE(K17:K22)</f>
-        <v>0.12147374352655282</v>
+        <v>0.12101008152308768</v>
       </c>
       <c r="L23" s="36">
         <f t="shared" si="0"/>
-        <v>0.39609373749623517</v>
+        <v>0.39348052943499806</v>
       </c>
       <c r="M23" s="36">
         <f t="shared" si="0"/>
-        <v>0.91198501872659132</v>
-      </c>
-      <c r="N23" s="93">
+        <v>0.90074906367041152</v>
+      </c>
+      <c r="N23" s="75">
         <f t="shared" si="0"/>
-        <v>0.73081193439024006</v>
+        <v>0.72867555133084816</v>
       </c>
     </row>
     <row r="25" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="87" t="s">
+      <c r="B25" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="87"/>
-      <c r="D25" s="87"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="87"/>
-      <c r="H25" s="87"/>
-      <c r="I25" s="87"/>
-      <c r="J25" s="87"/>
-      <c r="K25" s="87"/>
-      <c r="L25" s="87"/>
-      <c r="M25" s="87"/>
-      <c r="N25" s="87"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="76"/>
+      <c r="G25" s="76"/>
+      <c r="H25" s="76"/>
+      <c r="I25" s="76"/>
+      <c r="J25" s="76"/>
+      <c r="K25" s="76"/>
+      <c r="L25" s="76"/>
+      <c r="M25" s="76"/>
+      <c r="N25" s="76"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="28"/>
-      <c r="C26" s="69" t="s">
+      <c r="C26" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="69" t="s">
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="H26" s="70"/>
-      <c r="I26" s="70"/>
-      <c r="J26" s="71"/>
-      <c r="K26" s="69" t="s">
+      <c r="H26" s="78"/>
+      <c r="I26" s="78"/>
+      <c r="J26" s="79"/>
+      <c r="K26" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="L26" s="70"/>
-      <c r="M26" s="70"/>
-      <c r="N26" s="71"/>
+      <c r="L26" s="78"/>
+      <c r="M26" s="78"/>
+      <c r="N26" s="79"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="29" t="s">
@@ -2075,7 +2078,7 @@
       <c r="H28" s="26">
         <v>0.32771535580524302</v>
       </c>
-      <c r="I28" s="88">
+      <c r="I28" s="70">
         <v>0.39325842696629199</v>
       </c>
       <c r="J28" s="19">
@@ -2087,10 +2090,10 @@
       <c r="L28" s="26">
         <v>0.38350910834132301</v>
       </c>
-      <c r="M28" s="88">
+      <c r="M28" s="70">
         <v>0.898876404494382</v>
       </c>
-      <c r="N28" s="90">
+      <c r="N28" s="72">
         <v>0.71757145419661905</v>
       </c>
     </row>
@@ -2116,7 +2119,7 @@
       <c r="H29" s="26">
         <v>0.40566959921798601</v>
       </c>
-      <c r="I29" s="88">
+      <c r="I29" s="70">
         <v>0.93258426966292096</v>
       </c>
       <c r="J29" s="19">
@@ -2128,10 +2131,10 @@
       <c r="L29" s="26">
         <v>0.40060851926977598</v>
       </c>
-      <c r="M29" s="88">
+      <c r="M29" s="70">
         <v>0.88764044943820197</v>
       </c>
-      <c r="N29" s="90">
+      <c r="N29" s="72">
         <v>0.73719287597665695</v>
       </c>
     </row>
@@ -2157,7 +2160,7 @@
       <c r="H30" s="26">
         <v>0.39980256663376101</v>
       </c>
-      <c r="I30" s="88">
+      <c r="I30" s="70">
         <v>0.91011235955056102</v>
       </c>
       <c r="J30" s="19">
@@ -2169,10 +2172,10 @@
       <c r="L30" s="26">
         <v>0.401203610832497</v>
       </c>
-      <c r="M30" s="88">
+      <c r="M30" s="70">
         <v>0.898876404494382</v>
       </c>
-      <c r="N30" s="90">
+      <c r="N30" s="72">
         <v>0.73756818784008005</v>
       </c>
     </row>
@@ -2189,7 +2192,7 @@
       <c r="E31" s="56">
         <v>2.2471910112359501E-2</v>
       </c>
-      <c r="F31" s="86">
+      <c r="F31" s="69">
         <v>0.14990633779917201</v>
       </c>
       <c r="G31" s="54">
@@ -2198,7 +2201,7 @@
       <c r="H31" s="55">
         <v>0.248091603053435</v>
       </c>
-      <c r="I31" s="89">
+      <c r="I31" s="71">
         <v>0.29213483146067398</v>
       </c>
       <c r="J31" s="56">
@@ -2210,10 +2213,10 @@
       <c r="L31" s="55">
         <v>0.35747883349012199</v>
       </c>
-      <c r="M31" s="89">
+      <c r="M31" s="71">
         <v>0.85393258426966201</v>
       </c>
-      <c r="N31" s="91">
+      <c r="N31" s="73">
         <v>0.68901440157859695</v>
       </c>
     </row>
@@ -2230,7 +2233,7 @@
       <c r="E32" s="56">
         <v>3.3707865168539297E-2</v>
       </c>
-      <c r="F32" s="86">
+      <c r="F32" s="69">
         <v>0.18314425071961701</v>
       </c>
       <c r="G32" s="54">
@@ -2239,7 +2242,7 @@
       <c r="H32" s="55">
         <v>0.343749999999999</v>
       </c>
-      <c r="I32" s="89">
+      <c r="I32" s="71">
         <v>0.61797752808988704</v>
       </c>
       <c r="J32" s="56">
@@ -2251,10 +2254,10 @@
       <c r="L32" s="55">
         <v>0.38038038038038002</v>
       </c>
-      <c r="M32" s="89">
+      <c r="M32" s="71">
         <v>0.85393258426966201</v>
       </c>
-      <c r="N32" s="91">
+      <c r="N32" s="73">
         <v>0.71638039019274102</v>
       </c>
     </row>
@@ -2295,7 +2298,7 @@
       <c r="M33" s="39">
         <v>0.91011235955056102</v>
       </c>
-      <c r="N33" s="92">
+      <c r="N33" s="74">
         <v>0.72778520378537404</v>
       </c>
     </row>
@@ -2308,7 +2311,7 @@
         <v>0.42719298245614029</v>
       </c>
       <c r="D34" s="36">
-        <f t="shared" ref="D34:N34" si="1">AVERAGE(D28:D33)</f>
+        <f t="shared" ref="D34:F34" si="1">AVERAGE(D28:D33)</f>
         <v>2.4931472726465769E-2</v>
       </c>
       <c r="E34" s="36">
@@ -2324,7 +2327,7 @@
         <v>0.14183762742492401</v>
       </c>
       <c r="H34" s="36">
-        <f t="shared" ref="H34:N34" si="2">AVERAGE(H28:H33)</f>
+        <f t="shared" ref="H34:J34" si="2">AVERAGE(H28:H33)</f>
         <v>0.34724939470348831</v>
       </c>
       <c r="I34" s="36">
@@ -2347,13 +2350,777 @@
         <f t="shared" si="3"/>
         <v>0.88389513108614182</v>
       </c>
-      <c r="N34" s="93">
+      <c r="N34" s="75">
         <f t="shared" si="3"/>
         <v>0.72091875226167801</v>
       </c>
     </row>
+    <row r="36" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="76" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="76"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="76"/>
+      <c r="F36" s="76"/>
+      <c r="G36" s="76"/>
+      <c r="H36" s="76"/>
+      <c r="I36" s="76"/>
+      <c r="J36" s="76"/>
+      <c r="K36" s="76"/>
+      <c r="L36" s="76"/>
+      <c r="M36" s="76"/>
+      <c r="N36" s="76"/>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B37" s="28"/>
+      <c r="C37" s="77" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="78"/>
+      <c r="E37" s="78"/>
+      <c r="F37" s="79"/>
+      <c r="G37" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="H37" s="78"/>
+      <c r="I37" s="78"/>
+      <c r="J37" s="79"/>
+      <c r="K37" s="77" t="s">
+        <v>15</v>
+      </c>
+      <c r="L37" s="78"/>
+      <c r="M37" s="78"/>
+      <c r="N37" s="79"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B38" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="I38" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="J38" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="K38" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="L38" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="M38" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="N38" s="31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B39" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="D39" s="26">
+        <v>7.9787234042553196E-2</v>
+      </c>
+      <c r="E39" s="19">
+        <v>6.7415730337078594E-2</v>
+      </c>
+      <c r="F39" s="62">
+        <v>0.25836318613440501</v>
+      </c>
+      <c r="G39" s="18">
+        <v>0.19318181818181801</v>
+      </c>
+      <c r="H39" s="26">
+        <v>0.31954887218045103</v>
+      </c>
+      <c r="I39" s="70">
+        <v>0.38202247191011202</v>
+      </c>
+      <c r="J39" s="19">
+        <v>0.58638477877383899</v>
+      </c>
+      <c r="K39" s="18">
+        <v>0.12637362637362601</v>
+      </c>
+      <c r="L39" s="26">
+        <v>0.38248337028824803</v>
+      </c>
+      <c r="M39" s="70">
+        <v>0.77528089887640395</v>
+      </c>
+      <c r="N39" s="72">
+        <v>0.71765960252373695</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B40" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="18">
+        <v>1</v>
+      </c>
+      <c r="D40" s="26">
+        <v>1.40056022408963E-2</v>
+      </c>
+      <c r="E40" s="19">
+        <v>1.12359550561797E-2</v>
+      </c>
+      <c r="F40" s="62">
+        <v>0.105999788000636</v>
+      </c>
+      <c r="G40" s="18">
+        <v>0.12241887905604699</v>
+      </c>
+      <c r="H40" s="26">
+        <v>0.40135396518375199</v>
+      </c>
+      <c r="I40" s="70">
+        <v>0.93258426966292096</v>
+      </c>
+      <c r="J40" s="19">
+        <v>0.73626986853425602</v>
+      </c>
+      <c r="K40" s="18">
+        <v>0.121661721068249</v>
+      </c>
+      <c r="L40" s="26">
+        <v>0.39805825242718401</v>
+      </c>
+      <c r="M40" s="70">
+        <v>0.92134831460674105</v>
+      </c>
+      <c r="N40" s="72">
+        <v>0.73314883564450095</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B41" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="18">
+        <v>0</v>
+      </c>
+      <c r="D41" s="26">
+        <v>0</v>
+      </c>
+      <c r="E41" s="19">
+        <v>0</v>
+      </c>
+      <c r="F41" s="62">
+        <v>0</v>
+      </c>
+      <c r="G41" s="18">
+        <v>0.124812030075187</v>
+      </c>
+      <c r="H41" s="26">
+        <v>0.40646425073457398</v>
+      </c>
+      <c r="I41" s="70">
+        <v>0.93258426966292096</v>
+      </c>
+      <c r="J41" s="19">
+        <v>0.74204114061226201</v>
+      </c>
+      <c r="K41" s="18">
+        <v>0.124610591900311</v>
+      </c>
+      <c r="L41" s="26">
+        <v>0.400801603206412</v>
+      </c>
+      <c r="M41" s="70">
+        <v>0.898876404494382</v>
+      </c>
+      <c r="N41" s="72">
+        <v>0.737139244397089</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B42" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="54">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="D42" s="55">
+        <v>2.78551532033426E-2</v>
+      </c>
+      <c r="E42" s="56">
+        <v>2.2471910112359501E-2</v>
+      </c>
+      <c r="F42" s="69">
+        <v>0.14985358173989299</v>
+      </c>
+      <c r="G42" s="54">
+        <v>0.155555555555555</v>
+      </c>
+      <c r="H42" s="55">
+        <v>0.26119402985074602</v>
+      </c>
+      <c r="I42" s="71">
+        <v>0.31460674157303298</v>
+      </c>
+      <c r="J42" s="56">
+        <v>0.53005115407551995</v>
+      </c>
+      <c r="K42" s="54">
+        <v>9.7625329815303405E-2</v>
+      </c>
+      <c r="L42" s="55">
+        <v>0.33213644524236902</v>
+      </c>
+      <c r="M42" s="71">
+        <v>0.83146067415730296</v>
+      </c>
+      <c r="N42" s="73">
+        <v>0.656685703512495</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B43" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="54">
+        <v>0.27272727272727199</v>
+      </c>
+      <c r="D43" s="55">
+        <v>4.0871934604904597E-2</v>
+      </c>
+      <c r="E43" s="56">
+        <v>3.3707865168539297E-2</v>
+      </c>
+      <c r="F43" s="69">
+        <v>0.18307947821512599</v>
+      </c>
+      <c r="G43" s="54">
+        <v>0.13157894736842099</v>
+      </c>
+      <c r="H43" s="55">
+        <v>0.33967391304347799</v>
+      </c>
+      <c r="I43" s="71">
+        <v>0.56179775280898803</v>
+      </c>
+      <c r="J43" s="56">
+        <v>0.65675794483980798</v>
+      </c>
+      <c r="K43" s="54">
+        <v>0.12202380952380899</v>
+      </c>
+      <c r="L43" s="55">
+        <v>0.39883268482490197</v>
+      </c>
+      <c r="M43" s="71">
+        <v>0.92134831460674105</v>
+      </c>
+      <c r="N43" s="73">
+        <v>0.73403268025193102</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B44" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="38">
+        <v>0</v>
+      </c>
+      <c r="D44" s="39">
+        <v>0</v>
+      </c>
+      <c r="E44" s="40">
+        <v>0</v>
+      </c>
+      <c r="F44" s="63">
+        <v>0</v>
+      </c>
+      <c r="G44" s="38">
+        <v>0.140435835351089</v>
+      </c>
+      <c r="H44" s="39">
+        <v>0.37711313394018198</v>
+      </c>
+      <c r="I44" s="39">
+        <v>0.651685393258427</v>
+      </c>
+      <c r="J44" s="40">
+        <v>0.69919861094429603</v>
+      </c>
+      <c r="K44" s="38">
+        <v>0.11929307805596399</v>
+      </c>
+      <c r="L44" s="39">
+        <v>0.39130434782608697</v>
+      </c>
+      <c r="M44" s="39">
+        <v>0.91011235955056102</v>
+      </c>
+      <c r="N44" s="74">
+        <v>0.72602300942270204</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="35">
+        <f>AVERAGE(C39:C44)</f>
+        <v>0.37323232323232297</v>
+      </c>
+      <c r="D45" s="36">
+        <f t="shared" ref="D45:F45" si="4">AVERAGE(D39:D44)</f>
+        <v>2.708665401528278E-2</v>
+      </c>
+      <c r="E45" s="36">
+        <f t="shared" si="4"/>
+        <v>2.2471910112359519E-2</v>
+      </c>
+      <c r="F45" s="64">
+        <f t="shared" si="4"/>
+        <v>0.11621600568167667</v>
+      </c>
+      <c r="G45" s="35">
+        <f>AVERAGE(G39:G44)</f>
+        <v>0.14466384426468618</v>
+      </c>
+      <c r="H45" s="36">
+        <f t="shared" ref="H45:J45" si="5">AVERAGE(H39:H44)</f>
+        <v>0.35089136082219713</v>
+      </c>
+      <c r="I45" s="36">
+        <f t="shared" si="5"/>
+        <v>0.62921348314606707</v>
+      </c>
+      <c r="J45" s="64">
+        <f t="shared" si="5"/>
+        <v>0.65845058296333014</v>
+      </c>
+      <c r="K45" s="35">
+        <f>AVERAGE(K39:K44)</f>
+        <v>0.11859802612287706</v>
+      </c>
+      <c r="L45" s="36">
+        <f t="shared" ref="L45:N45" si="6">AVERAGE(L39:L44)</f>
+        <v>0.38393611730253369</v>
+      </c>
+      <c r="M45" s="36">
+        <f t="shared" si="6"/>
+        <v>0.87640449438202195</v>
+      </c>
+      <c r="N45" s="75">
+        <f t="shared" si="6"/>
+        <v>0.71744817929207594</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47" s="76"/>
+      <c r="D47" s="76"/>
+      <c r="E47" s="76"/>
+      <c r="F47" s="76"/>
+      <c r="G47" s="76"/>
+      <c r="H47" s="76"/>
+      <c r="I47" s="76"/>
+      <c r="J47" s="76"/>
+      <c r="K47" s="76"/>
+      <c r="L47" s="76"/>
+      <c r="M47" s="76"/>
+      <c r="N47" s="76"/>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B48" s="28"/>
+      <c r="C48" s="77" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="78"/>
+      <c r="E48" s="78"/>
+      <c r="F48" s="79"/>
+      <c r="G48" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="H48" s="78"/>
+      <c r="I48" s="78"/>
+      <c r="J48" s="79"/>
+      <c r="K48" s="77" t="s">
+        <v>15</v>
+      </c>
+      <c r="L48" s="78"/>
+      <c r="M48" s="78"/>
+      <c r="N48" s="79"/>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B49" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E49" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F49" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="G49" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="H49" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="I49" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="J49" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="K49" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="L49" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="M49" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="N49" s="31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B50" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="18">
+        <v>0.27272727272727199</v>
+      </c>
+      <c r="D50" s="26">
+        <v>7.9365079365079305E-2</v>
+      </c>
+      <c r="E50" s="19">
+        <v>6.7415730337078594E-2</v>
+      </c>
+      <c r="F50" s="62">
+        <v>0.25817949383522498</v>
+      </c>
+      <c r="G50" s="18">
+        <v>0.18061674008810499</v>
+      </c>
+      <c r="H50" s="26">
+        <v>0.35162950257289799</v>
+      </c>
+      <c r="I50" s="70">
+        <v>0.46067415730337002</v>
+      </c>
+      <c r="J50" s="19">
+        <v>0.63275176444195502</v>
+      </c>
+      <c r="K50" s="18">
+        <v>0.105670103092783</v>
+      </c>
+      <c r="L50" s="26">
+        <v>0.36219081272084802</v>
+      </c>
+      <c r="M50" s="70">
+        <v>0.92134831460674105</v>
+      </c>
+      <c r="N50" s="72">
+        <v>0.68656567871447705</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B51" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="18">
+        <v>1</v>
+      </c>
+      <c r="D51" s="26">
+        <v>1.40056022408963E-2</v>
+      </c>
+      <c r="E51" s="19">
+        <v>1.12359550561797E-2</v>
+      </c>
+      <c r="F51" s="62">
+        <v>0.105999788000636</v>
+      </c>
+      <c r="G51" s="18">
+        <v>0.123695976154992</v>
+      </c>
+      <c r="H51" s="26">
+        <v>0.40408958130477102</v>
+      </c>
+      <c r="I51" s="70">
+        <v>0.93258426966292096</v>
+      </c>
+      <c r="J51" s="19">
+        <v>0.73938307425316196</v>
+      </c>
+      <c r="K51" s="18">
+        <v>0.12241887905604699</v>
+      </c>
+      <c r="L51" s="26">
+        <v>0.40135396518375199</v>
+      </c>
+      <c r="M51" s="70">
+        <v>0.93258426966292096</v>
+      </c>
+      <c r="N51" s="72">
+        <v>0.73626986853425602</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B52" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="D52" s="26">
+        <v>1.38888888888888E-2</v>
+      </c>
+      <c r="E52" s="19">
+        <v>1.12359550561797E-2</v>
+      </c>
+      <c r="F52" s="62">
+        <v>0.105887836072198</v>
+      </c>
+      <c r="G52" s="18">
+        <v>0.122137404580152</v>
+      </c>
+      <c r="H52" s="26">
+        <v>0.39564787339267998</v>
+      </c>
+      <c r="I52" s="70">
+        <v>0.898876404494382</v>
+      </c>
+      <c r="J52" s="19">
+        <v>0.731540092234368</v>
+      </c>
+      <c r="K52" s="18">
+        <v>0.126365054602184</v>
+      </c>
+      <c r="L52" s="26">
+        <v>0.40621865596790302</v>
+      </c>
+      <c r="M52" s="70">
+        <v>0.91011235955056102</v>
+      </c>
+      <c r="N52" s="72">
+        <v>0.74259503787027303</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B53" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="54">
+        <v>0</v>
+      </c>
+      <c r="D53" s="55">
+        <v>0</v>
+      </c>
+      <c r="E53" s="56">
+        <v>0</v>
+      </c>
+      <c r="F53" s="69">
+        <v>0</v>
+      </c>
+      <c r="G53" s="54">
+        <v>0.14285714285714199</v>
+      </c>
+      <c r="H53" s="55">
+        <v>0.25362318840579701</v>
+      </c>
+      <c r="I53" s="71">
+        <v>0.31460674157303298</v>
+      </c>
+      <c r="J53" s="56">
+        <v>0.52669901829205801</v>
+      </c>
+      <c r="K53" s="54">
+        <v>9.4805194805194795E-2</v>
+      </c>
+      <c r="L53" s="55">
+        <v>0.32415630550621599</v>
+      </c>
+      <c r="M53" s="71">
+        <v>0.82022471910112305</v>
+      </c>
+      <c r="N53" s="73">
+        <v>0.64645555376243602</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B54" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" s="54">
+        <v>0.214285714285714</v>
+      </c>
+      <c r="D54" s="55">
+        <v>4.0540540540540501E-2</v>
+      </c>
+      <c r="E54" s="56">
+        <v>3.3707865168539297E-2</v>
+      </c>
+      <c r="F54" s="69">
+        <v>0.182885023058592</v>
+      </c>
+      <c r="G54" s="54">
+        <v>0.13136729222520099</v>
+      </c>
+      <c r="H54" s="55">
+        <v>0.33607681755829899</v>
+      </c>
+      <c r="I54" s="71">
+        <v>0.550561797752809</v>
+      </c>
+      <c r="J54" s="56">
+        <v>0.65194252699486899</v>
+      </c>
+      <c r="K54" s="54">
+        <v>0.123475609756097</v>
+      </c>
+      <c r="L54" s="55">
+        <v>0.40019762845849799</v>
+      </c>
+      <c r="M54" s="71">
+        <v>0.91011235955056102</v>
+      </c>
+      <c r="N54" s="73">
+        <v>0.73609801852613099</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B55" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="38">
+        <v>0</v>
+      </c>
+      <c r="D55" s="39">
+        <v>0</v>
+      </c>
+      <c r="E55" s="40">
+        <v>0</v>
+      </c>
+      <c r="F55" s="63">
+        <v>0</v>
+      </c>
+      <c r="G55" s="38">
+        <v>0.14047619047619</v>
+      </c>
+      <c r="H55" s="39">
+        <v>0.38015463917525699</v>
+      </c>
+      <c r="I55" s="39">
+        <v>0.66292134831460603</v>
+      </c>
+      <c r="J55" s="40">
+        <v>0.70321300875949899</v>
+      </c>
+      <c r="K55" s="38">
+        <v>0.120058565153733</v>
+      </c>
+      <c r="L55" s="39">
+        <v>0.39461020211741998</v>
+      </c>
+      <c r="M55" s="39">
+        <v>0.92134831460674105</v>
+      </c>
+      <c r="N55" s="74">
+        <v>0.72915827711658998</v>
+      </c>
+    </row>
+    <row r="56" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" s="35">
+        <f>AVERAGE(C50:C55)</f>
+        <v>0.28950216450216432</v>
+      </c>
+      <c r="D56" s="36">
+        <f t="shared" ref="D56:F56" si="7">AVERAGE(D50:D55)</f>
+        <v>2.4633351839234152E-2</v>
+      </c>
+      <c r="E56" s="36">
+        <f t="shared" si="7"/>
+        <v>2.0599250936329552E-2</v>
+      </c>
+      <c r="F56" s="64">
+        <f t="shared" si="7"/>
+        <v>0.10882535682777517</v>
+      </c>
+      <c r="G56" s="35">
+        <f>AVERAGE(G50:G55)</f>
+        <v>0.14019179106363033</v>
+      </c>
+      <c r="H56" s="36">
+        <f t="shared" ref="H56:J56" si="8">AVERAGE(H50:H55)</f>
+        <v>0.35353693373495032</v>
+      </c>
+      <c r="I56" s="36">
+        <f t="shared" si="8"/>
+        <v>0.63670411985018682</v>
+      </c>
+      <c r="J56" s="64">
+        <f t="shared" si="8"/>
+        <v>0.66425491416265181</v>
+      </c>
+      <c r="K56" s="35">
+        <f>AVERAGE(K50:K55)</f>
+        <v>0.1154655677443398</v>
+      </c>
+      <c r="L56" s="36">
+        <f t="shared" ref="L56:N56" si="9">AVERAGE(L50:L55)</f>
+        <v>0.3814545949924395</v>
+      </c>
+      <c r="M56" s="36">
+        <f t="shared" si="9"/>
+        <v>0.90262172284644127</v>
+      </c>
+      <c r="N56" s="75">
+        <f t="shared" si="9"/>
+        <v>0.71285707242069385</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="19">
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="G48:J48"/>
+    <mergeCell ref="K48:N48"/>
+    <mergeCell ref="B36:N36"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="K37:N37"/>
+    <mergeCell ref="B47:N47"/>
     <mergeCell ref="B25:N25"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="G26:J26"/>
@@ -2375,8 +3142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89318DEB-50A8-45CC-801F-03E6368A0566}">
   <dimension ref="B1:P70"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="L66" sqref="L66:P66"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2386,46 +3153,46 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="74"/>
-      <c r="P2" s="75"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="87"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="76" t="s">
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="76" t="s">
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="79"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="90"/>
+      <c r="P3" s="91"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -2476,46 +3243,46 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
-        <v>0.46428571428571402</v>
+        <v>0.44</v>
       </c>
       <c r="C5" s="21">
-        <v>9.6726190476190396E-2</v>
+        <v>8.2212257100149497E-2</v>
       </c>
       <c r="D5" s="2">
-        <v>8.0745341614906804E-2</v>
+        <v>6.8322981366459604E-2</v>
       </c>
       <c r="E5" s="42">
-        <v>0.28332255345124002</v>
+        <v>0.26067010125345702</v>
       </c>
       <c r="F5" s="6">
         <v>1</v>
       </c>
       <c r="G5" s="7">
-        <v>0.53846153846153799</v>
+        <v>0.45833333333333298</v>
       </c>
       <c r="H5" s="21">
-        <v>0.104477611940298</v>
+        <v>8.2335329341317307E-2</v>
       </c>
       <c r="I5" s="2">
-        <v>8.6956521739130405E-2</v>
+        <v>6.8322981366459604E-2</v>
       </c>
       <c r="J5" s="42">
-        <v>0.29419115353221598</v>
+        <v>0.260721348693499</v>
       </c>
       <c r="K5" s="6">
         <v>0.1</v>
       </c>
       <c r="L5" s="7">
-        <v>0.201086956521739</v>
+        <v>0.19277108433734899</v>
       </c>
       <c r="M5" s="21">
-        <v>0.223429951690821</v>
+        <v>0.19753086419752999</v>
       </c>
       <c r="N5" s="2">
-        <v>0.229813664596273</v>
+        <v>0.19875776397515499</v>
       </c>
       <c r="O5" s="42">
-        <v>0.46540503916466802</v>
+        <v>0.43398367607058402</v>
       </c>
       <c r="P5" s="6">
         <v>0.1</v>
@@ -2523,16 +3290,16 @@
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
-        <v>0.26229508196721302</v>
+        <v>0.28571428571428498</v>
       </c>
       <c r="C6" s="21">
-        <v>0.113475177304964</v>
+        <v>0.114285714285714</v>
       </c>
       <c r="D6" s="2">
         <v>9.9378881987577605E-2</v>
       </c>
       <c r="E6" s="42">
-        <v>0.31245789801818702</v>
+        <v>0.31276870869686302</v>
       </c>
       <c r="F6" s="6">
         <v>2</v>
@@ -2553,16 +3320,16 @@
         <v>0.2</v>
       </c>
       <c r="L6" s="7">
-        <v>0.183856502242152</v>
+        <v>0.143442622950819</v>
       </c>
       <c r="M6" s="21">
-        <v>0.23644752018454401</v>
+        <v>0.197072072072072</v>
       </c>
       <c r="N6" s="2">
-        <v>0.25465838509316702</v>
+        <v>0.217391304347826</v>
       </c>
       <c r="O6" s="42">
-        <v>0.48634609516764399</v>
+        <v>0.44679136025294097</v>
       </c>
       <c r="P6" s="6">
         <v>0.2</v>
@@ -2570,16 +3337,16 @@
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
-        <v>0.26373626373626302</v>
+        <v>0.25301204819277101</v>
       </c>
       <c r="C7" s="21">
-        <v>0.163265306122448</v>
+        <v>0.14442916093534999</v>
       </c>
       <c r="D7" s="2">
-        <v>0.14906832298136599</v>
+        <v>0.13043478260869501</v>
       </c>
       <c r="E7" s="42">
-        <v>0.381001769223693</v>
+        <v>0.356752167420477</v>
       </c>
       <c r="F7" s="6">
         <v>3</v>
@@ -2600,16 +3367,16 @@
         <v>0.3</v>
       </c>
       <c r="L7" s="7">
-        <v>0.15444015444015399</v>
+        <v>0.14642857142857099</v>
       </c>
       <c r="M7" s="21">
-        <v>0.22148394241417399</v>
+        <v>0.22186147186147101</v>
       </c>
       <c r="N7" s="2">
-        <v>0.24844720496894401</v>
+        <v>0.25465838509316702</v>
       </c>
       <c r="O7" s="42">
-        <v>0.47662184891840798</v>
+        <v>0.48047449849287499</v>
       </c>
       <c r="P7" s="6">
         <v>0.3</v>
@@ -2617,46 +3384,46 @@
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
-        <v>0.21621621621621601</v>
+        <v>0.23529411764705799</v>
       </c>
       <c r="C8" s="21">
-        <v>0.158940397350993</v>
+        <v>0.18348623853210999</v>
       </c>
       <c r="D8" s="2">
-        <v>0.14906832298136599</v>
+        <v>0.17391304347826</v>
       </c>
       <c r="E8" s="42">
-        <v>0.379468556689258</v>
+        <v>0.40954087116362098</v>
       </c>
       <c r="F8" s="6">
         <v>4</v>
       </c>
       <c r="G8" s="7">
-        <v>0.53846153846153799</v>
+        <v>0.48275862068965503</v>
       </c>
       <c r="H8" s="21">
-        <v>0.104477611940298</v>
+        <v>0.10401188707280801</v>
       </c>
       <c r="I8" s="2">
         <v>8.6956521739130405E-2</v>
       </c>
       <c r="J8" s="42">
-        <v>0.29419115353221598</v>
+        <v>0.29401770879657402</v>
       </c>
       <c r="K8" s="6">
         <v>0.4</v>
       </c>
       <c r="L8" s="7">
-        <v>0.162454873646209</v>
+        <v>0.13818181818181799</v>
       </c>
       <c r="M8" s="21">
-        <v>0.2442996742671</v>
+        <v>0.206746463547334</v>
       </c>
       <c r="N8" s="2">
-        <v>0.27950310559006197</v>
+        <v>0.23602484472049601</v>
       </c>
       <c r="O8" s="42">
-        <v>0.50412639115838298</v>
+        <v>0.46276178620012498</v>
       </c>
       <c r="P8" s="6">
         <v>0.4</v>
@@ -2664,16 +3431,16 @@
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
-        <v>0.183098591549295</v>
+        <v>0.21768707482993099</v>
       </c>
       <c r="C9" s="21">
-        <v>0.165394402035623</v>
+        <v>0.20227560050568799</v>
       </c>
       <c r="D9" s="2">
-        <v>0.161490683229813</v>
+        <v>0.19875776397515499</v>
       </c>
       <c r="E9" s="42">
-        <v>0.39263793924574902</v>
+        <v>0.43568189898253501</v>
       </c>
       <c r="F9" s="6">
         <v>5</v>
@@ -2693,19 +3460,19 @@
       <c r="K9" s="6">
         <v>0.5</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="18">
         <v>0.16501650165016499</v>
       </c>
-      <c r="M9" s="22">
+      <c r="M9" s="26">
         <v>0.263991552270327</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="19">
         <v>0.31055900621117999</v>
       </c>
-      <c r="O9" s="43">
+      <c r="O9" s="45">
         <v>0.52899057891551104</v>
       </c>
-      <c r="P9" s="12">
+      <c r="P9" s="92">
         <v>0.5</v>
       </c>
     </row>
@@ -2740,34 +3507,34 @@
       <c r="K10" s="6">
         <v>0.6</v>
       </c>
-      <c r="L10" s="7">
-        <v>0.163636363636363</v>
-      </c>
-      <c r="M10" s="21">
-        <v>0.24483133841131599</v>
-      </c>
-      <c r="N10" s="2">
-        <v>0.27950310559006197</v>
-      </c>
-      <c r="O10" s="42">
-        <v>0.50434317310396803</v>
-      </c>
-      <c r="P10" s="6">
+      <c r="L10" s="8">
+        <v>0.18181818181818099</v>
+      </c>
+      <c r="M10" s="22">
+        <v>0.29411764705882298</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0.34782608695652101</v>
+      </c>
+      <c r="O10" s="43">
+        <v>0.55995248500681205</v>
+      </c>
+      <c r="P10" s="12">
         <v>0.6</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
-        <v>0.19786096256684399</v>
+        <v>0.20689655172413701</v>
       </c>
       <c r="C11" s="21">
-        <v>0.22262334536702699</v>
+        <v>0.22004889975550099</v>
       </c>
       <c r="D11" s="2">
-        <v>0.229813664596273</v>
+        <v>0.223602484472049</v>
       </c>
       <c r="E11" s="42">
-        <v>0.46511527777568001</v>
+        <v>0.459929093656813</v>
       </c>
       <c r="F11" s="6">
         <v>7</v>
@@ -2805,16 +3572,16 @@
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
-        <v>0.19251336898395699</v>
+        <v>0.197044334975369</v>
       </c>
       <c r="C12" s="21">
-        <v>0.21660649819494501</v>
+        <v>0.23612750885478101</v>
       </c>
       <c r="D12" s="2">
-        <v>0.223602484472049</v>
+        <v>0.24844720496894401</v>
       </c>
       <c r="E12" s="42">
-        <v>0.45869157134409599</v>
+        <v>0.48229611840990599</v>
       </c>
       <c r="F12" s="6">
         <v>8</v>
@@ -2846,22 +3613,22 @@
       <c r="O12" s="45">
         <v>0.52553534547604996</v>
       </c>
-      <c r="P12" s="80">
+      <c r="P12" s="6">
         <v>0.8</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="8">
-        <v>0.19480519480519401</v>
+        <v>0.20091324200913199</v>
       </c>
       <c r="C13" s="22">
-        <v>0.25714285714285701</v>
+        <v>0.25492468134414797</v>
       </c>
       <c r="D13" s="3">
-        <v>0.27950310559006197</v>
+        <v>0.27329192546583803</v>
       </c>
       <c r="E13" s="43">
-        <v>0.50908902181158</v>
+        <v>0.50456708326768296</v>
       </c>
       <c r="F13" s="12">
         <v>9</v>
@@ -2889,16 +3656,16 @@
     </row>
     <row r="14" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="9">
-        <v>0.17333333333333301</v>
+        <v>0.18534482758620599</v>
       </c>
       <c r="C14" s="23">
-        <v>0.22439585730724901</v>
+        <v>0.24543378995433701</v>
       </c>
       <c r="D14" s="10">
-        <v>0.24223602484472001</v>
+        <v>0.26708074534161402</v>
       </c>
       <c r="E14" s="44">
-        <v>0.47393608694829498</v>
+        <v>0.49733242450595899</v>
       </c>
       <c r="F14" s="11">
         <v>10</v>
@@ -2926,46 +3693,46 @@
     </row>
     <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="73"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="73"/>
-      <c r="N16" s="73"/>
-      <c r="O16" s="74"/>
-      <c r="P16" s="75"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="85"/>
+      <c r="F16" s="85"/>
+      <c r="G16" s="85"/>
+      <c r="H16" s="85"/>
+      <c r="I16" s="85"/>
+      <c r="J16" s="85"/>
+      <c r="K16" s="85"/>
+      <c r="L16" s="85"/>
+      <c r="M16" s="85"/>
+      <c r="N16" s="85"/>
+      <c r="O16" s="86"/>
+      <c r="P16" s="87"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="76" t="s">
+      <c r="B17" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="79"/>
-      <c r="G17" s="76" t="s">
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="91"/>
+      <c r="G17" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="77"/>
-      <c r="I17" s="77"/>
-      <c r="J17" s="78"/>
-      <c r="K17" s="79"/>
-      <c r="L17" s="76" t="s">
+      <c r="H17" s="89"/>
+      <c r="I17" s="89"/>
+      <c r="J17" s="90"/>
+      <c r="K17" s="91"/>
+      <c r="L17" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="77"/>
-      <c r="N17" s="77"/>
-      <c r="O17" s="78"/>
-      <c r="P17" s="79"/>
+      <c r="M17" s="89"/>
+      <c r="N17" s="89"/>
+      <c r="O17" s="90"/>
+      <c r="P17" s="91"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
@@ -3466,46 +4233,46 @@
     </row>
     <row r="29" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="72" t="s">
+      <c r="B30" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="73"/>
-      <c r="D30" s="73"/>
-      <c r="E30" s="73"/>
-      <c r="F30" s="73"/>
-      <c r="G30" s="73"/>
-      <c r="H30" s="73"/>
-      <c r="I30" s="73"/>
-      <c r="J30" s="73"/>
-      <c r="K30" s="73"/>
-      <c r="L30" s="73"/>
-      <c r="M30" s="73"/>
-      <c r="N30" s="73"/>
-      <c r="O30" s="74"/>
-      <c r="P30" s="75"/>
+      <c r="C30" s="85"/>
+      <c r="D30" s="85"/>
+      <c r="E30" s="85"/>
+      <c r="F30" s="85"/>
+      <c r="G30" s="85"/>
+      <c r="H30" s="85"/>
+      <c r="I30" s="85"/>
+      <c r="J30" s="85"/>
+      <c r="K30" s="85"/>
+      <c r="L30" s="85"/>
+      <c r="M30" s="85"/>
+      <c r="N30" s="85"/>
+      <c r="O30" s="86"/>
+      <c r="P30" s="87"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="76" t="s">
+      <c r="B31" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="77"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="76" t="s">
+      <c r="C31" s="89"/>
+      <c r="D31" s="89"/>
+      <c r="E31" s="90"/>
+      <c r="F31" s="91"/>
+      <c r="G31" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="H31" s="77"/>
-      <c r="I31" s="77"/>
-      <c r="J31" s="78"/>
-      <c r="K31" s="79"/>
-      <c r="L31" s="76" t="s">
+      <c r="H31" s="89"/>
+      <c r="I31" s="89"/>
+      <c r="J31" s="90"/>
+      <c r="K31" s="91"/>
+      <c r="L31" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="M31" s="77"/>
-      <c r="N31" s="77"/>
-      <c r="O31" s="78"/>
-      <c r="P31" s="79"/>
+      <c r="M31" s="89"/>
+      <c r="N31" s="89"/>
+      <c r="O31" s="90"/>
+      <c r="P31" s="91"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
@@ -3665,16 +4432,16 @@
         <v>3</v>
       </c>
       <c r="G35" s="7">
-        <v>0.161434977578475</v>
+        <v>0.15909090909090901</v>
       </c>
       <c r="H35" s="21">
-        <v>0.207612456747404</v>
+        <v>0.202546296296296</v>
       </c>
       <c r="I35" s="2">
-        <v>0.223602484472049</v>
+        <v>0.217391304347826</v>
       </c>
       <c r="J35" s="42">
-        <v>0.45524703019962198</v>
+        <v>0.44906898602469297</v>
       </c>
       <c r="K35" s="6">
         <v>0.3</v>
@@ -3727,16 +4494,16 @@
         <v>0.4</v>
       </c>
       <c r="L36" s="7">
-        <v>0.123560209424083</v>
+        <v>0.12381951731374601</v>
       </c>
       <c r="M36" s="21">
-        <v>0.36898061288305101</v>
+        <v>0.36944270507200899</v>
       </c>
       <c r="N36" s="2">
         <v>0.73291925465838503</v>
       </c>
       <c r="O36" s="42">
-        <v>0.70214518998473696</v>
+        <v>0.70255329533159405</v>
       </c>
       <c r="P36" s="6">
         <v>0.4</v>
@@ -3744,31 +4511,31 @@
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" s="7">
-        <v>0.15609756097560901</v>
+        <v>0.16336633663366301</v>
       </c>
       <c r="C37" s="21">
-        <v>0.18845700824499401</v>
+        <v>0.195035460992907</v>
       </c>
       <c r="D37" s="2">
-        <v>0.19875776397515499</v>
+        <v>0.20496894409937799</v>
       </c>
       <c r="E37" s="42">
-        <v>0.43047686144875702</v>
+        <v>0.43751790331961499</v>
       </c>
       <c r="F37" s="6">
         <v>5</v>
       </c>
       <c r="G37" s="7">
-        <v>0.13594040968342599</v>
+        <v>0.13754646840148699</v>
       </c>
       <c r="H37" s="21">
-        <v>0.30906011854360699</v>
+        <v>0.31302876480541397</v>
       </c>
       <c r="I37" s="2">
-        <v>0.453416149068323</v>
+        <v>0.45962732919254601</v>
       </c>
       <c r="J37" s="42">
-        <v>0.60921100811226503</v>
+        <v>0.61336949330303503</v>
       </c>
       <c r="K37" s="6">
         <v>0.5</v>
@@ -3838,16 +4605,16 @@
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="7">
-        <v>0.140388768898488</v>
+        <v>0.138528138528138</v>
       </c>
       <c r="C39" s="21">
-        <v>0.29358626919602498</v>
+        <v>0.28933092224231399</v>
       </c>
       <c r="D39" s="2">
-        <v>0.40372670807453398</v>
+        <v>0.39751552795030998</v>
       </c>
       <c r="E39" s="42">
-        <v>0.58385458821948999</v>
+        <v>0.57934599110796803</v>
       </c>
       <c r="F39" s="6">
         <v>7</v>
@@ -3868,16 +4635,16 @@
         <v>0.7</v>
       </c>
       <c r="L39" s="8">
-        <v>0.12698412698412601</v>
+        <v>0.126872246696035</v>
       </c>
       <c r="M39" s="22">
-        <v>0.40494938132733399</v>
+        <v>0.404721753794266</v>
       </c>
       <c r="N39" s="3">
         <v>0.894409937888198</v>
       </c>
       <c r="O39" s="43">
-        <v>0.74035061630875598</v>
+        <v>0.74011434675868004</v>
       </c>
       <c r="P39" s="12">
         <v>0.7</v>
@@ -3915,16 +4682,16 @@
         <v>0.8</v>
       </c>
       <c r="L40" s="7">
-        <v>0.125868055555555</v>
+        <v>0.12597741094700199</v>
       </c>
       <c r="M40" s="21">
-        <v>0.40367483296213802</v>
+        <v>0.40389972144846797</v>
       </c>
       <c r="N40" s="2">
         <v>0.90062111801242195</v>
       </c>
       <c r="O40" s="42">
-        <v>0.73887597965041596</v>
+        <v>0.73911428830994297</v>
       </c>
       <c r="P40" s="6">
         <v>0.8</v>
@@ -3932,16 +4699,16 @@
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="18">
-        <v>0.13490959666203001</v>
+        <v>0.13509749303621099</v>
       </c>
       <c r="C41" s="26">
-        <v>0.35583272193690302</v>
+        <v>0.356093979441997</v>
       </c>
       <c r="D41" s="19">
         <v>0.60248447204968902</v>
       </c>
       <c r="E41" s="45">
-        <v>0.67522427897169601</v>
+        <v>0.67539873299320097</v>
       </c>
       <c r="F41" s="6">
         <v>9</v>
@@ -4006,46 +4773,46 @@
     </row>
     <row r="43" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="72" t="s">
+      <c r="B44" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="C44" s="73"/>
-      <c r="D44" s="73"/>
-      <c r="E44" s="73"/>
-      <c r="F44" s="73"/>
-      <c r="G44" s="73"/>
-      <c r="H44" s="73"/>
-      <c r="I44" s="73"/>
-      <c r="J44" s="73"/>
-      <c r="K44" s="73"/>
-      <c r="L44" s="73"/>
-      <c r="M44" s="73"/>
-      <c r="N44" s="73"/>
-      <c r="O44" s="74"/>
-      <c r="P44" s="75"/>
+      <c r="C44" s="85"/>
+      <c r="D44" s="85"/>
+      <c r="E44" s="85"/>
+      <c r="F44" s="85"/>
+      <c r="G44" s="85"/>
+      <c r="H44" s="85"/>
+      <c r="I44" s="85"/>
+      <c r="J44" s="85"/>
+      <c r="K44" s="85"/>
+      <c r="L44" s="85"/>
+      <c r="M44" s="85"/>
+      <c r="N44" s="85"/>
+      <c r="O44" s="86"/>
+      <c r="P44" s="87"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B45" s="76" t="s">
+      <c r="B45" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="77"/>
-      <c r="D45" s="77"/>
-      <c r="E45" s="78"/>
-      <c r="F45" s="79"/>
-      <c r="G45" s="76" t="s">
+      <c r="C45" s="89"/>
+      <c r="D45" s="89"/>
+      <c r="E45" s="90"/>
+      <c r="F45" s="91"/>
+      <c r="G45" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="H45" s="77"/>
-      <c r="I45" s="77"/>
-      <c r="J45" s="78"/>
-      <c r="K45" s="79"/>
-      <c r="L45" s="76" t="s">
+      <c r="H45" s="89"/>
+      <c r="I45" s="89"/>
+      <c r="J45" s="90"/>
+      <c r="K45" s="91"/>
+      <c r="L45" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="M45" s="77"/>
-      <c r="N45" s="77"/>
-      <c r="O45" s="78"/>
-      <c r="P45" s="79"/>
+      <c r="M45" s="89"/>
+      <c r="N45" s="89"/>
+      <c r="O45" s="90"/>
+      <c r="P45" s="91"/>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
@@ -4096,46 +4863,46 @@
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B47" s="18">
-        <v>0.77777777777777701</v>
+        <v>0.85714285714285698</v>
       </c>
       <c r="C47" s="26">
-        <v>5.3598774885145403E-2</v>
+        <v>4.60829493087557E-2</v>
       </c>
       <c r="D47" s="19">
+        <v>3.7267080745341602E-2</v>
+      </c>
+      <c r="E47" s="45">
+        <v>0.19300908323805499</v>
+      </c>
+      <c r="F47" s="6">
+        <v>1</v>
+      </c>
+      <c r="G47" s="7">
+        <v>0.63636363636363602</v>
+      </c>
+      <c r="H47" s="21">
+        <v>5.3435114503816702E-2</v>
+      </c>
+      <c r="I47" s="2">
         <v>4.3478260869565202E-2</v>
       </c>
-      <c r="E47" s="45">
-        <v>0.20843285159979499</v>
-      </c>
-      <c r="F47" s="80">
-        <v>1</v>
-      </c>
-      <c r="G47" s="7">
-        <v>0.66666666666666596</v>
-      </c>
-      <c r="H47" s="21">
-        <v>6.0975609756097497E-2</v>
-      </c>
-      <c r="I47" s="2">
-        <v>4.9689440993788803E-2</v>
-      </c>
       <c r="J47" s="42">
-        <v>0.22273686302766499</v>
+        <v>0.20835125721358</v>
       </c>
       <c r="K47" s="6">
         <v>0.1</v>
       </c>
       <c r="L47" s="7">
-        <v>0.3</v>
+        <v>0.27272727272727199</v>
       </c>
       <c r="M47" s="21">
-        <v>0.16574585635359099</v>
+        <v>0.14563106796116501</v>
       </c>
       <c r="N47" s="2">
-        <v>0.14906832298136599</v>
+        <v>0.13043478260869501</v>
       </c>
       <c r="O47" s="42">
-        <v>0.381842411999047</v>
+        <v>0.357180870359953</v>
       </c>
       <c r="P47" s="6">
         <v>0.1</v>
@@ -4143,46 +4910,46 @@
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B48" s="7">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="C48" s="21">
-        <v>5.3680981595091999E-2</v>
+        <v>4.6153846153846101E-2</v>
       </c>
       <c r="D48" s="2">
-        <v>4.3478260869565202E-2</v>
+        <v>3.7267080745341602E-2</v>
       </c>
       <c r="E48" s="42">
-        <v>0.20847363681720901</v>
+        <v>0.19304683562633601</v>
       </c>
       <c r="F48" s="6">
         <v>2</v>
       </c>
       <c r="G48" s="7">
-        <v>0.66666666666666596</v>
+        <v>0.52941176470588203</v>
       </c>
       <c r="H48" s="21">
-        <v>6.0975609756097497E-2</v>
+        <v>6.8078668683812404E-2</v>
       </c>
       <c r="I48" s="2">
-        <v>4.9689440993788803E-2</v>
+        <v>5.5900621118012403E-2</v>
       </c>
       <c r="J48" s="42">
-        <v>0.22273686302766499</v>
+        <v>0.23606297194318501</v>
       </c>
       <c r="K48" s="6">
         <v>0.2</v>
       </c>
       <c r="L48" s="7">
-        <v>0.184782608695652</v>
+        <v>0.18848167539267</v>
       </c>
       <c r="M48" s="21">
-        <v>0.205314009661835</v>
+        <v>0.215568862275449</v>
       </c>
       <c r="N48" s="2">
-        <v>0.21118012422360199</v>
+        <v>0.223602484472049</v>
       </c>
       <c r="O48" s="42">
-        <v>0.44586070831448898</v>
+        <v>0.45831012298594198</v>
       </c>
       <c r="P48" s="6">
         <v>0.2</v>
@@ -4190,46 +4957,46 @@
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B49" s="7">
-        <v>0.77777777777777701</v>
+        <v>0.8</v>
       </c>
       <c r="C49" s="21">
-        <v>5.3598774885145403E-2</v>
+        <v>6.11620795107033E-2</v>
       </c>
       <c r="D49" s="2">
-        <v>4.3478260869565202E-2</v>
+        <v>4.9689440993788803E-2</v>
       </c>
       <c r="E49" s="42">
-        <v>0.20843285159979499</v>
+        <v>0.222824091095637</v>
       </c>
       <c r="F49" s="6">
         <v>3</v>
       </c>
       <c r="G49" s="7">
-        <v>0.5625</v>
+        <v>0.58823529411764697</v>
       </c>
       <c r="H49" s="21">
-        <v>6.8181818181818094E-2</v>
+        <v>7.5642965204235996E-2</v>
       </c>
       <c r="I49" s="2">
-        <v>5.5900621118012403E-2</v>
+        <v>6.2111801242236003E-2</v>
       </c>
       <c r="J49" s="42">
-        <v>0.236109272418661</v>
+        <v>0.24888102584271399</v>
       </c>
       <c r="K49" s="6">
         <v>0.3</v>
       </c>
       <c r="L49" s="7">
-        <v>0.16055045871559601</v>
+        <v>0.16734693877550999</v>
       </c>
       <c r="M49" s="21">
-        <v>0.20301624129930301</v>
+        <v>0.23059617547806499</v>
       </c>
       <c r="N49" s="2">
-        <v>0.217391304347826</v>
+        <v>0.25465838509316702</v>
       </c>
       <c r="O49" s="42">
-        <v>0.4492582669545</v>
+        <v>0.48408830409866799</v>
       </c>
       <c r="P49" s="6">
         <v>0.3</v>
@@ -4237,266 +5004,266 @@
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50" s="7">
-        <v>0.875</v>
+        <v>0.85714285714285698</v>
       </c>
       <c r="C50" s="21">
-        <v>5.3680981595091999E-2</v>
+        <v>4.60829493087557E-2</v>
       </c>
       <c r="D50" s="2">
-        <v>4.3478260869565202E-2</v>
+        <v>3.7267080745341602E-2</v>
       </c>
       <c r="E50" s="42">
-        <v>0.20847363681720901</v>
+        <v>0.19300908323805499</v>
       </c>
       <c r="F50" s="6">
         <v>4</v>
       </c>
-      <c r="G50" s="7">
-        <v>0.56521739130434701</v>
-      </c>
-      <c r="H50" s="21">
-        <v>9.7451274362818502E-2</v>
-      </c>
-      <c r="I50" s="2">
-        <v>8.0745341614906804E-2</v>
-      </c>
-      <c r="J50" s="42">
-        <v>0.28360105794535201</v>
-      </c>
-      <c r="K50" s="6">
+      <c r="G50" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="H50" s="22">
+        <v>9.0361445783132502E-2</v>
+      </c>
+      <c r="I50" s="3">
+        <v>7.4534161490683204E-2</v>
+      </c>
+      <c r="J50" s="43">
+        <v>0.27258204079420201</v>
+      </c>
+      <c r="K50" s="12">
         <v>0.4</v>
       </c>
       <c r="L50" s="7">
-        <v>0.15983606557377</v>
+        <v>0.16666666666666599</v>
       </c>
       <c r="M50" s="21">
-        <v>0.21959459459459399</v>
+        <v>0.24617067833698</v>
       </c>
       <c r="N50" s="2">
-        <v>0.24223602484472001</v>
+        <v>0.27950310559006197</v>
       </c>
       <c r="O50" s="42">
-        <v>0.47203332476946402</v>
+        <v>0.50488472074532997</v>
       </c>
       <c r="P50" s="6">
         <v>0.4</v>
       </c>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B51" s="7">
-        <v>0.85714285714285698</v>
-      </c>
-      <c r="C51" s="21">
-        <v>4.60829493087557E-2</v>
-      </c>
-      <c r="D51" s="2">
-        <v>3.7267080745341602E-2</v>
-      </c>
-      <c r="E51" s="42">
-        <v>0.19300908323805499</v>
-      </c>
-      <c r="F51" s="6">
+      <c r="B51" s="8">
+        <v>0.88888888888888795</v>
+      </c>
+      <c r="C51" s="22">
+        <v>6.1255742725880503E-2</v>
+      </c>
+      <c r="D51" s="3">
+        <v>4.9689440993788803E-2</v>
+      </c>
+      <c r="E51" s="43">
+        <v>0.22286769232706799</v>
+      </c>
+      <c r="F51" s="12">
         <v>5</v>
       </c>
       <c r="G51" s="7">
-        <v>0.5</v>
+        <v>0.42105263157894701</v>
       </c>
       <c r="H51" s="21">
-        <v>8.2582582582582595E-2</v>
+        <v>6.0331825037707301E-2</v>
       </c>
       <c r="I51" s="2">
-        <v>6.8322981366459604E-2</v>
+        <v>4.9689440993788803E-2</v>
       </c>
       <c r="J51" s="42">
-        <v>0.26082381336583499</v>
+        <v>0.222431295408792</v>
       </c>
       <c r="K51" s="6">
         <v>0.5</v>
       </c>
       <c r="L51" s="18">
-        <v>0.15753424657534201</v>
+        <v>0.16838487972508501</v>
       </c>
       <c r="M51" s="26">
-        <v>0.24572649572649499</v>
+        <v>0.26203208556149699</v>
       </c>
       <c r="N51" s="19">
-        <v>0.28571428571428498</v>
+        <v>0.30434782608695599</v>
       </c>
       <c r="O51" s="45">
-        <v>0.50816012887311901</v>
-      </c>
-      <c r="P51" s="80">
+        <v>0.52492255696068302</v>
+      </c>
+      <c r="P51" s="6">
         <v>0.5</v>
       </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" s="7">
-        <v>0.63636363636363602</v>
+        <v>0.83333333333333304</v>
       </c>
       <c r="C52" s="21">
-        <v>5.3435114503816702E-2</v>
+        <v>3.8461538461538401E-2</v>
       </c>
       <c r="D52" s="2">
-        <v>4.3478260869565202E-2</v>
+        <v>3.1055900621118002E-2</v>
       </c>
       <c r="E52" s="42">
-        <v>0.20835125721358</v>
+        <v>0.17619238115479199</v>
       </c>
       <c r="F52" s="6">
         <v>6</v>
       </c>
       <c r="G52" s="18">
-        <v>0.44444444444444398</v>
+        <v>0.45454545454545398</v>
       </c>
       <c r="H52" s="26">
-        <v>8.9418777943368097E-2</v>
+        <v>7.5075075075075007E-2</v>
       </c>
       <c r="I52" s="19">
-        <v>7.4534161490683204E-2</v>
+        <v>6.2111801242236003E-2</v>
       </c>
       <c r="J52" s="45">
-        <v>0.27220750449294101</v>
+        <v>0.24863690511124201</v>
       </c>
       <c r="K52" s="6">
         <v>0.6</v>
       </c>
       <c r="L52" s="18">
-        <v>0.163701067615658</v>
+        <v>0.17114093959731499</v>
       </c>
       <c r="M52" s="26">
-        <v>0.248648648648648</v>
+        <v>0.27070063694267499</v>
       </c>
       <c r="N52" s="19">
-        <v>0.28571428571428498</v>
+        <v>0.31677018633540299</v>
       </c>
       <c r="O52" s="45">
-        <v>0.50936807469798995</v>
+        <v>0.53494948772130801</v>
       </c>
       <c r="P52" s="6">
         <v>0.6</v>
       </c>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B53" s="8">
-        <v>0.875</v>
-      </c>
-      <c r="C53" s="22">
-        <v>5.3680981595091999E-2</v>
-      </c>
-      <c r="D53" s="3">
-        <v>4.3478260869565202E-2</v>
-      </c>
-      <c r="E53" s="43">
-        <v>0.20847363681720901</v>
-      </c>
-      <c r="F53" s="12">
+      <c r="B53" s="18">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="C53" s="26">
+        <v>3.0721966205837101E-2</v>
+      </c>
+      <c r="D53" s="19">
+        <v>2.4844720496894401E-2</v>
+      </c>
+      <c r="E53" s="45">
+        <v>0.15752958906504</v>
+      </c>
+      <c r="F53" s="92">
         <v>7</v>
       </c>
       <c r="G53" s="7">
-        <v>0.44</v>
+        <v>0.42857142857142799</v>
       </c>
       <c r="H53" s="21">
-        <v>8.2212257100149497E-2</v>
+        <v>6.7669172932330796E-2</v>
       </c>
       <c r="I53" s="2">
-        <v>6.8322981366459604E-2</v>
+        <v>5.5900621118012403E-2</v>
       </c>
       <c r="J53" s="42">
-        <v>0.26067010125345702</v>
+        <v>0.235877679158006</v>
       </c>
       <c r="K53" s="6">
         <v>0.7</v>
       </c>
-      <c r="L53" s="18">
-        <v>0.149837133550488</v>
-      </c>
-      <c r="M53" s="26">
-        <v>0.24185068349106201</v>
-      </c>
-      <c r="N53" s="19">
-        <v>0.28571428571428498</v>
-      </c>
-      <c r="O53" s="45">
-        <v>0.506508287481504</v>
-      </c>
-      <c r="P53" s="6">
+      <c r="L53" s="8">
+        <v>0.16927899686520301</v>
+      </c>
+      <c r="M53" s="22">
+        <v>0.28037383177570002</v>
+      </c>
+      <c r="N53" s="3">
+        <v>0.335403726708074</v>
+      </c>
+      <c r="O53" s="43">
+        <v>0.54830964393270298</v>
+      </c>
+      <c r="P53" s="12">
         <v>0.7</v>
       </c>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54" s="7">
-        <v>0.85714285714285698</v>
+        <v>0.875</v>
       </c>
       <c r="C54" s="21">
-        <v>4.60829493087557E-2</v>
+        <v>5.3680981595091999E-2</v>
       </c>
       <c r="D54" s="2">
-        <v>3.7267080745341602E-2</v>
+        <v>4.3478260869565202E-2</v>
       </c>
       <c r="E54" s="42">
-        <v>0.19300908323805499</v>
+        <v>0.20847363681720901</v>
       </c>
       <c r="F54" s="6">
         <v>8</v>
       </c>
       <c r="G54" s="7">
-        <v>0.48148148148148101</v>
+        <v>0.39285714285714202</v>
       </c>
       <c r="H54" s="21">
-        <v>9.6870342771982101E-2</v>
+        <v>8.1845238095238096E-2</v>
       </c>
       <c r="I54" s="2">
-        <v>8.0745341614906804E-2</v>
+        <v>6.8322981366459604E-2</v>
       </c>
       <c r="J54" s="42">
-        <v>0.283378276247226</v>
+        <v>0.26051629844652602</v>
       </c>
       <c r="K54" s="6">
         <v>0.8</v>
       </c>
-      <c r="L54" s="8">
-        <v>0.14626865671641701</v>
-      </c>
-      <c r="M54" s="22">
-        <v>0.25025536261491299</v>
-      </c>
-      <c r="N54" s="3">
+      <c r="L54" s="18">
+        <v>0.144542772861356</v>
+      </c>
+      <c r="M54" s="26">
+        <v>0.24923702950152499</v>
+      </c>
+      <c r="N54" s="19">
         <v>0.30434782608695599</v>
       </c>
-      <c r="O54" s="43">
-        <v>0.51991016079755403</v>
-      </c>
-      <c r="P54" s="12">
+      <c r="O54" s="45">
+        <v>0.51945209008236604</v>
+      </c>
+      <c r="P54" s="92">
         <v>0.8</v>
       </c>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B55" s="18">
-        <v>0.85714285714285698</v>
+        <v>0.875</v>
       </c>
       <c r="C55" s="26">
-        <v>4.60829493087557E-2</v>
+        <v>5.3680981595091999E-2</v>
       </c>
       <c r="D55" s="19">
-        <v>3.7267080745341602E-2</v>
+        <v>4.3478260869565202E-2</v>
       </c>
       <c r="E55" s="45">
-        <v>0.19300908323805499</v>
+        <v>0.20847363681720901</v>
       </c>
       <c r="F55" s="6">
         <v>9</v>
       </c>
       <c r="G55" s="18">
-        <v>0.41935483870967699</v>
+        <v>0.42857142857142799</v>
       </c>
       <c r="H55" s="26">
-        <v>9.6296296296296199E-2</v>
+        <v>8.9285714285714302E-2</v>
       </c>
       <c r="I55" s="19">
-        <v>8.0745341614906804E-2</v>
+        <v>7.4534161490683204E-2</v>
       </c>
       <c r="J55" s="45">
-        <v>0.28315531926837501</v>
+        <v>0.272153957230794</v>
       </c>
       <c r="K55" s="6">
         <v>0.9</v>
@@ -4508,34 +5275,34 @@
       <c r="P55" s="14"/>
     </row>
     <row r="56" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="81">
-        <v>0.83333333333333304</v>
-      </c>
-      <c r="C56" s="82">
-        <v>3.8461538461538401E-2</v>
-      </c>
-      <c r="D56" s="83">
+      <c r="B56" s="65">
+        <v>0.625</v>
+      </c>
+      <c r="C56" s="66">
+        <v>3.8343558282208499E-2</v>
+      </c>
+      <c r="D56" s="67">
         <v>3.1055900621118002E-2</v>
       </c>
-      <c r="E56" s="84">
-        <v>0.17619238115479199</v>
-      </c>
-      <c r="F56" s="85">
+      <c r="E56" s="68">
+        <v>0.176123434808519</v>
+      </c>
+      <c r="F56" s="11">
         <v>10</v>
       </c>
-      <c r="G56" s="48">
-        <v>0.46666666666666601</v>
-      </c>
-      <c r="H56" s="49">
-        <v>0.103857566765578</v>
-      </c>
-      <c r="I56" s="50">
-        <v>8.6956521739130405E-2</v>
-      </c>
-      <c r="J56" s="51">
-        <v>0.29395987114305999</v>
-      </c>
-      <c r="K56" s="52">
+      <c r="G56" s="65">
+        <v>0.42857142857142799</v>
+      </c>
+      <c r="H56" s="66">
+        <v>8.9285714285714302E-2</v>
+      </c>
+      <c r="I56" s="67">
+        <v>7.4534161490683204E-2</v>
+      </c>
+      <c r="J56" s="68">
+        <v>0.272153957230794</v>
+      </c>
+      <c r="K56" s="11">
         <v>1</v>
       </c>
       <c r="L56" s="15"/>
@@ -4546,46 +5313,46 @@
     </row>
     <row r="57" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="72" t="s">
+      <c r="B58" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="73"/>
-      <c r="D58" s="73"/>
-      <c r="E58" s="73"/>
-      <c r="F58" s="73"/>
-      <c r="G58" s="73"/>
-      <c r="H58" s="73"/>
-      <c r="I58" s="73"/>
-      <c r="J58" s="73"/>
-      <c r="K58" s="73"/>
-      <c r="L58" s="73"/>
-      <c r="M58" s="73"/>
-      <c r="N58" s="73"/>
-      <c r="O58" s="74"/>
-      <c r="P58" s="75"/>
+      <c r="C58" s="85"/>
+      <c r="D58" s="85"/>
+      <c r="E58" s="85"/>
+      <c r="F58" s="85"/>
+      <c r="G58" s="85"/>
+      <c r="H58" s="85"/>
+      <c r="I58" s="85"/>
+      <c r="J58" s="85"/>
+      <c r="K58" s="85"/>
+      <c r="L58" s="85"/>
+      <c r="M58" s="85"/>
+      <c r="N58" s="85"/>
+      <c r="O58" s="86"/>
+      <c r="P58" s="87"/>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B59" s="76" t="s">
+      <c r="B59" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="C59" s="77"/>
-      <c r="D59" s="77"/>
-      <c r="E59" s="78"/>
-      <c r="F59" s="79"/>
-      <c r="G59" s="76" t="s">
+      <c r="C59" s="89"/>
+      <c r="D59" s="89"/>
+      <c r="E59" s="90"/>
+      <c r="F59" s="91"/>
+      <c r="G59" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="H59" s="77"/>
-      <c r="I59" s="77"/>
-      <c r="J59" s="78"/>
-      <c r="K59" s="79"/>
-      <c r="L59" s="76" t="s">
+      <c r="H59" s="89"/>
+      <c r="I59" s="89"/>
+      <c r="J59" s="90"/>
+      <c r="K59" s="91"/>
+      <c r="L59" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="M59" s="77"/>
-      <c r="N59" s="77"/>
-      <c r="O59" s="78"/>
-      <c r="P59" s="79"/>
+      <c r="M59" s="89"/>
+      <c r="N59" s="89"/>
+      <c r="O59" s="90"/>
+      <c r="P59" s="91"/>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
@@ -4639,7 +5406,7 @@
       <c r="C61" s="26"/>
       <c r="D61" s="19"/>
       <c r="E61" s="45"/>
-      <c r="F61" s="80">
+      <c r="F61" s="6">
         <v>1</v>
       </c>
       <c r="G61" s="7">
@@ -4678,7 +5445,7 @@
       <c r="C62" s="26"/>
       <c r="D62" s="19"/>
       <c r="E62" s="45"/>
-      <c r="F62" s="80">
+      <c r="F62" s="6">
         <v>2</v>
       </c>
       <c r="G62" s="7">
@@ -4717,7 +5484,7 @@
       <c r="C63" s="26"/>
       <c r="D63" s="19"/>
       <c r="E63" s="45"/>
-      <c r="F63" s="80">
+      <c r="F63" s="6">
         <v>3</v>
       </c>
       <c r="G63" s="7">
@@ -4756,7 +5523,7 @@
       <c r="C64" s="26"/>
       <c r="D64" s="19"/>
       <c r="E64" s="45"/>
-      <c r="F64" s="80">
+      <c r="F64" s="6">
         <v>4</v>
       </c>
       <c r="G64" s="7">
@@ -4795,7 +5562,7 @@
       <c r="C65" s="26"/>
       <c r="D65" s="19"/>
       <c r="E65" s="45"/>
-      <c r="F65" s="80">
+      <c r="F65" s="6">
         <v>5</v>
       </c>
       <c r="G65" s="7">
@@ -4825,7 +5592,7 @@
       <c r="O65" s="45">
         <v>0.62674974357786495</v>
       </c>
-      <c r="P65" s="80">
+      <c r="P65" s="6">
         <v>0.5</v>
       </c>
     </row>
@@ -4834,7 +5601,7 @@
       <c r="C66" s="26"/>
       <c r="D66" s="19"/>
       <c r="E66" s="45"/>
-      <c r="F66" s="80">
+      <c r="F66" s="6">
         <v>6</v>
       </c>
       <c r="G66" s="18">
@@ -4873,7 +5640,7 @@
       <c r="C67" s="26"/>
       <c r="D67" s="19"/>
       <c r="E67" s="45"/>
-      <c r="F67" s="80">
+      <c r="F67" s="6">
         <v>7</v>
       </c>
       <c r="G67" s="7">
@@ -4912,7 +5679,7 @@
       <c r="C68" s="26"/>
       <c r="D68" s="19"/>
       <c r="E68" s="45"/>
-      <c r="F68" s="80">
+      <c r="F68" s="6">
         <v>8</v>
       </c>
       <c r="G68" s="7">
@@ -4951,7 +5718,7 @@
       <c r="C69" s="26"/>
       <c r="D69" s="19"/>
       <c r="E69" s="45"/>
-      <c r="F69" s="80">
+      <c r="F69" s="6">
         <v>9</v>
       </c>
       <c r="G69" s="18">
@@ -4976,11 +5743,11 @@
       <c r="P69" s="14"/>
     </row>
     <row r="70" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="81"/>
-      <c r="C70" s="82"/>
-      <c r="D70" s="83"/>
-      <c r="E70" s="84"/>
-      <c r="F70" s="85">
+      <c r="B70" s="65"/>
+      <c r="C70" s="66"/>
+      <c r="D70" s="67"/>
+      <c r="E70" s="68"/>
+      <c r="F70" s="11">
         <v>10</v>
       </c>
       <c r="G70" s="48">
@@ -5006,6 +5773,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B30:P30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="G31:K31"/>
+    <mergeCell ref="L31:P31"/>
     <mergeCell ref="B58:P58"/>
     <mergeCell ref="B59:F59"/>
     <mergeCell ref="G59:K59"/>
@@ -5022,10 +5793,6 @@
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="G3:K3"/>
     <mergeCell ref="L3:P3"/>
-    <mergeCell ref="B30:P30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="G31:K31"/>
-    <mergeCell ref="L31:P31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>